<commit_message>
Added a column of doing to 3D model list
</commit_message>
<xml_diff>
--- a/Project Work/3D models/3D Models.xlsx
+++ b/Project Work/3D models/3D Models.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>What?</t>
   </si>
@@ -79,15 +79,31 @@
   </si>
   <si>
     <t>Trash Cans</t>
+  </si>
+  <si>
+    <t>Doing</t>
+  </si>
+  <si>
+    <t>Frederik</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -131,10 +147,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,116 +431,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="18.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="3"/>
+    <col min="3" max="3" width="13.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="B14" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
lots of little changes to the room
</commit_message>
<xml_diff>
--- a/Project Work/3D models/3D Models.xlsx
+++ b/Project Work/3D models/3D Models.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>What?</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>lul</t>
+  </si>
+  <si>
+    <t>Oliver</t>
   </si>
 </sst>
 </file>
@@ -140,10 +143,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,7 +431,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,6 +543,9 @@
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B13" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">

</xml_diff>

<commit_message>
added my name to model design sheet
</commit_message>
<xml_diff>
--- a/Project Work/3D models/3D Models.xlsx
+++ b/Project Work/3D models/3D Models.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>What?</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Oliver</t>
+  </si>
+  <si>
+    <t>Niclas</t>
   </si>
 </sst>
 </file>
@@ -143,11 +146,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,7 +433,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,6 +530,9 @@
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -543,7 +548,7 @@
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>